<commit_message>
Support PTP: PtpClock, ExtClk and SyncE; update Inits
</commit_message>
<xml_diff>
--- a/Docs/BOM.ETX2i100G.xlsx
+++ b/Docs/BOM.ETX2i100G.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\ate\AutoTesters\TCL\ETX-2-100G\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0236B40E-2E66-4962-80D2-BA9274967771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17DACB1-2CA1-4BC6-9290-CBD6E2A3C4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="1470" windowWidth="21315" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7410" yWindow="1350" windowWidth="17025" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="OLE_LINK4" localSheetId="0">Sheet1!$A$21</definedName>
+    <definedName name="OLE_LINK4" localSheetId="0">Sheet1!$A$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -530,29 +530,6 @@
   </si>
   <si>
     <t>AT-ETX-2I-100G</t>
-  </si>
-  <si>
-    <r>
-      <t>RM-34 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>for ATE-PIO-USB, ATE-RELAY-BOX-4, AUX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <t>2 units</t>
@@ -578,6 +555,50 @@
   <si>
     <t>ETX-2I-10G-8SFPP as AUX
 ETX-2I-10G-B/19/AC/8SFPP 6251830000</t>
+  </si>
+  <si>
+    <t>AT-ETX2i100G/CBL03</t>
+  </si>
+  <si>
+    <t>CBL-RJ45/D9/F/6FT</t>
+  </si>
+  <si>
+    <t>CBL-MP-28</t>
+  </si>
+  <si>
+    <t>ETX-205A/AC/19/PTP</t>
+  </si>
+  <si>
+    <t>CNT-91</t>
+  </si>
+  <si>
+    <t>RM-35/P1 (for CNT-91)</t>
+  </si>
+  <si>
+    <r>
+      <t>RM-34 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>for ATE-PIO-USB, ATE-RELAY-BOX-4, AUX*3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>AT-ETX2i100G/CBL04</t>
   </si>
 </sst>
 </file>
@@ -658,7 +679,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -945,11 +966,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1017,6 +1092,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1026,41 +1137,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1342,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,129 +1459,129 @@
     <row r="4" spans="1:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="39"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B6" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="9">
-        <v>1</v>
-      </c>
-      <c r="C7" s="10">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="40">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="C7" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="40">
+        <v>1</v>
+      </c>
+      <c r="C8" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="40">
+        <v>1</v>
+      </c>
+      <c r="C9" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6">
-        <f t="shared" ref="C10" si="0">B10*2</f>
+      <c r="B12" s="38"/>
+      <c r="C12" s="39"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" ref="C13" si="0">B13*2</f>
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+    <row r="14" spans="1:3" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="9">
-        <v>1</v>
-      </c>
-      <c r="C11" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="30"/>
-    </row>
-    <row r="15" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="33"/>
+    </row>
+    <row r="18" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="B15" s="4">
-        <v>2</v>
-      </c>
-      <c r="C15" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="4">
-        <v>1</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="4">
-        <v>2</v>
-      </c>
-      <c r="C17" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>38</v>
       </c>
       <c r="B18" s="4">
         <v>2</v>
@@ -1501,323 +1592,400 @@
     </row>
     <row r="19" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="4">
         <v>2</v>
       </c>
       <c r="C19" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="4">
+        <v>2</v>
+      </c>
+      <c r="C20" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+    <row r="21" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="4">
+        <v>2</v>
+      </c>
+      <c r="C21" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="4">
+        <v>2</v>
+      </c>
+      <c r="C22" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2</v>
+      </c>
+      <c r="C23" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="4">
+        <v>5</v>
+      </c>
+      <c r="C24" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="9">
-        <v>2</v>
-      </c>
-      <c r="C22" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="27"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="6">
-        <v>1</v>
-      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="33"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
+      <c r="C28" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="4">
-        <v>1</v>
-      </c>
-      <c r="C26" s="6">
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="C33" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="9">
-        <v>1</v>
-      </c>
-      <c r="C27" s="10">
+      <c r="B34" s="9">
+        <v>1</v>
+      </c>
+      <c r="C34" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="14"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+    <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="15"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="33"/>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="B36" s="26"/>
+      <c r="C36" s="27"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="36"/>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="B37" s="29"/>
+      <c r="C37" s="30"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="4">
-        <v>1</v>
-      </c>
-      <c r="C31" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="30"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="4">
-        <v>1</v>
-      </c>
-      <c r="C33" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="C34" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="4">
-        <v>1</v>
-      </c>
-      <c r="C35" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="4">
-        <v>0</v>
-      </c>
-      <c r="C36" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="9">
-        <v>2</v>
-      </c>
-      <c r="C37" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="38"/>
-      <c r="C39" s="39"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="33"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B40" s="4">
         <v>1</v>
       </c>
-      <c r="C40" s="6"/>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C40" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B41" s="4">
         <v>1</v>
       </c>
-      <c r="C41" s="6"/>
+      <c r="C41" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
       </c>
-      <c r="C42" s="6"/>
-    </row>
-    <row r="43" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="9">
-        <v>1</v>
-      </c>
-      <c r="C43" s="10"/>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
+      <c r="C42" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0</v>
+      </c>
+      <c r="C43" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="9">
+        <v>2</v>
+      </c>
+      <c r="C44" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="16"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
     </row>
-    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="21"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48" s="38"/>
-      <c r="C48" s="39"/>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="35"/>
+      <c r="C46" s="36"/>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1</v>
+      </c>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1</v>
+      </c>
+      <c r="C48" s="6"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="4">
+        <v>1</v>
+      </c>
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="9">
+        <v>1</v>
+      </c>
+      <c r="C50" s="10"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="20"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="20"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="20"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="23"/>
+      <c r="B54" s="21"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" s="35"/>
+      <c r="C55" s="36"/>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B49" s="4">
-        <v>1</v>
-      </c>
-      <c r="C49" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+      <c r="B56" s="4">
+        <v>1</v>
+      </c>
+      <c r="C56" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="4">
-        <v>1</v>
-      </c>
-      <c r="C50" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+      <c r="B57" s="4">
+        <v>1</v>
+      </c>
+      <c r="C57" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B51" s="4">
-        <v>1</v>
-      </c>
-      <c r="C51" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+      <c r="B58" s="4">
+        <v>1</v>
+      </c>
+      <c r="C58" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B52" s="4">
-        <v>1</v>
-      </c>
-      <c r="C52" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
+      <c r="B59" s="4">
+        <v>1</v>
+      </c>
+      <c r="C59" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B53" s="9">
-        <v>1</v>
-      </c>
-      <c r="C53" s="10">
+      <c r="B60" s="9">
+        <v>1</v>
+      </c>
+      <c r="C60" s="10">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:C37"/>
     <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A55:C55"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>